<commit_message>
Antenna Distance Sheet Updated
</commit_message>
<xml_diff>
--- a/Notes/Planet Distances.xlsx
+++ b/Notes/Planet Distances.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RealismOverhaul\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan paplaczyk\Dropbox\GAMES\KSP\Git\RealismOverhaul\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E43173-2282-4FA1-9EAF-7310E2BFD43E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="DSN">Sheet1!$T$12</definedName>
     <definedName name="Type">Sheet1!$T$14</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Mercury</t>
   </si>
@@ -123,15 +122,21 @@
   </si>
   <si>
     <t>CB</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Flyby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -182,7 +187,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -316,47 +321,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P12" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:P12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P12" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:P12"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CB"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Pe" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Avg" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Ap" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Closest" dataDxfId="11">
+    <tableColumn id="1" name="CB"/>
+    <tableColumn id="2" name="Pe" dataDxfId="14"/>
+    <tableColumn id="3" name="Avg" dataDxfId="13"/>
+    <tableColumn id="4" name="Ap" dataDxfId="12"/>
+    <tableColumn id="5" name="Closest" dataDxfId="11">
       <calculatedColumnFormula>B2-$R$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Avg2" dataDxfId="10">
+    <tableColumn id="6" name="Avg2" dataDxfId="10">
       <calculatedColumnFormula>(E2+G2)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Furthest" dataDxfId="9">
+    <tableColumn id="7" name="Furthest" dataDxfId="9">
       <calculatedColumnFormula>$R$5+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="KM Close" dataDxfId="8" dataCellStyle="Comma">
+    <tableColumn id="8" name="KM Close" dataDxfId="8" dataCellStyle="Comma">
       <calculatedColumnFormula>E2*$R$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="KM Avg" dataDxfId="7" dataCellStyle="Comma">
+    <tableColumn id="9" name="KM Avg" dataDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>F2*$R$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="KM Far" dataDxfId="6" dataCellStyle="Comma">
+    <tableColumn id="10" name="KM Far" dataDxfId="6" dataCellStyle="Comma">
       <calculatedColumnFormula>G2*$R$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Gm Close" dataDxfId="5">
+    <tableColumn id="11" name="Gm Close" dataDxfId="5">
       <calculatedColumnFormula>H2/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Gm Avg" dataDxfId="4">
+    <tableColumn id="12" name="Gm Avg" dataDxfId="4">
       <calculatedColumnFormula>I2/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Gm Far" dataDxfId="3">
+    <tableColumn id="13" name="Gm Far" dataDxfId="3">
       <calculatedColumnFormula>J2/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Tm Close" dataDxfId="2">
+    <tableColumn id="14" name="Tm Close" dataDxfId="2">
       <calculatedColumnFormula>H2/1000000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Tm Avg" dataDxfId="1">
+    <tableColumn id="15" name="Tm Avg" dataDxfId="1">
       <calculatedColumnFormula>I2/1000000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Tm Far" dataDxfId="0">
+    <tableColumn id="16" name="Tm Far" dataDxfId="0">
       <calculatedColumnFormula>J2/1000000000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -626,11 +631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1417,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="R13" s="2"/>
       <c r="T13" s="2">
-        <v>450000</v>
+        <v>25000000000</v>
       </c>
       <c r="U13" t="s">
         <v>27</v>
@@ -1430,14 +1435,14 @@
       <c r="H15" s="3"/>
       <c r="R15" s="6">
         <f>MIN(MIN(DSN,Antenna)+SQRT(DSN*Antenna),IF(Type="Omni",Antenna*100,Antenna*1000))</f>
-        <v>450000000</v>
+        <v>1713194301613.4133</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H16" s="3"/>
       <c r="R16" s="6" t="str">
         <f>IF(R15&gt;1000000000000000,R15/1000000000000000&amp;" Pm",IF(R15&gt;1000000000000,R15/1000000000000&amp;" Tm",IF(R15&gt;1000000000,R15/1000000000&amp;" Gm",R15/1000000&amp;" Mm")))</f>
-        <v>450 Mm</v>
+        <v>1.71319430161341 Tm</v>
       </c>
       <c r="T16" s="2"/>
     </row>
@@ -1472,6 +1477,13 @@
       </c>
     </row>
     <row r="21" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f>1550800</f>
+        <v>1550800</v>
+      </c>
+      <c r="M21" t="s">
+        <v>31</v>
+      </c>
       <c r="T21" s="2">
         <f t="shared" ref="T21:T30" si="21">T20*10</f>
         <v>100000000</v>
@@ -1481,6 +1493,12 @@
       </c>
     </row>
     <row r="22" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>9700000</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
       <c r="T22" s="2">
         <f t="shared" si="21"/>
         <v>1000000000</v>
@@ -1490,6 +1508,10 @@
       </c>
     </row>
     <row r="23" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f>L21*4</f>
+        <v>6203200</v>
+      </c>
       <c r="T23" s="2">
         <f t="shared" si="21"/>
         <v>10000000000</v>
@@ -1499,6 +1521,10 @@
       </c>
     </row>
     <row r="24" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f>L23/1000</f>
+        <v>6203.2</v>
+      </c>
       <c r="T24" s="2">
         <f t="shared" si="21"/>
         <v>100000000000</v>

</xml_diff>